<commit_message>
update web_form testing (requirements)
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -452,6 +452,133 @@
   </si>
   <si>
     <t>S-9</t>
+  </si>
+  <si>
+    <t>Поле Email</t>
+  </si>
+  <si>
+    <t>E-1</t>
+  </si>
+  <si>
+    <t>E-2</t>
+  </si>
+  <si>
+    <t>E-3</t>
+  </si>
+  <si>
+    <t>E-4</t>
+  </si>
+  <si>
+    <t>E-5</t>
+  </si>
+  <si>
+    <t>E-6</t>
+  </si>
+  <si>
+    <t>E-7</t>
+  </si>
+  <si>
+    <t>E-8</t>
+  </si>
+  <si>
+    <t>E-9</t>
+  </si>
+  <si>
+    <t>Your email address. *</t>
+  </si>
+  <si>
+    <t>Обязательна</t>
+  </si>
+  <si>
+    <t>N-10</t>
+  </si>
+  <si>
+    <t>Возможность оставить поле пустым</t>
+  </si>
+  <si>
+    <t>Обязательно для заполнения</t>
+  </si>
+  <si>
+    <t>S-10</t>
+  </si>
+  <si>
+    <t>Не обязательно для заполнения</t>
+  </si>
+  <si>
+    <t>E-10</t>
+  </si>
+  <si>
+    <t>Доменные зоны</t>
+  </si>
+  <si>
+    <t>Допустимы все доменные зоны</t>
+  </si>
+  <si>
+    <t>E-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Имя почтового ящика (до @): латинские буквы, арабские цифры, символы: " . ", " - ", "_"
+Имя домена (после @ и до последней . ): латинские буквы, арабские цифры, символы: " . ", " - ", "_"
+Имя домена (после последней . ): латинские буквы
+Примечание: запрещено введение 2 и более символов подряд, а также расположение символов в начале и в конце поля </t>
+  </si>
+  <si>
+    <t>Имя почтового ящика (до @) - 1
+Имя домена (после @ и до последней . ) - 2
+Имя домена (после последней . ) - 2</t>
+  </si>
+  <si>
+    <t>Имя почтового ящика (до @) - 32
+Имя домена (после @ и до последней . ) - 24
+Имя домена (после последней . ) - 16</t>
+  </si>
+  <si>
+    <t>Поле Password</t>
+  </si>
+  <si>
+    <t>P-1</t>
+  </si>
+  <si>
+    <t>P-2</t>
+  </si>
+  <si>
+    <t>P-3</t>
+  </si>
+  <si>
+    <t>P-4</t>
+  </si>
+  <si>
+    <t>P-5</t>
+  </si>
+  <si>
+    <t>P-6</t>
+  </si>
+  <si>
+    <t>P-7</t>
+  </si>
+  <si>
+    <t>P-8</t>
+  </si>
+  <si>
+    <t>P-9</t>
+  </si>
+  <si>
+    <t>P-10</t>
+  </si>
+  <si>
+    <t>Enter a password. *</t>
+  </si>
+  <si>
+    <t>Должна присутствовать как минимум 1 буква в верхнем регистре</t>
+  </si>
+  <si>
+    <t>Допустимы буквы только в нижнем регистре</t>
+  </si>
+  <si>
+    <t>Латинские буквы, арабские цифры, "@"
+Примечание:  
+1.В поле обязательно должны присутствовать: 1 буква в вернем регистре, 1 цифра, 1  @;
+2. Запрещено введение 2 и более  "@" подряд.</t>
   </si>
 </sst>
 </file>
@@ -502,7 +629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -657,11 +784,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -737,6 +895,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1068,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,85 +1698,85 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C49" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="16"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="B50" s="15"/>
+      <c r="C50" s="16"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>124</v>
@@ -1608,21 +1784,21 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>107</v>
@@ -1630,63 +1806,332 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="B56" s="7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="19">
+      <c r="C59" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B58" s="7" t="s">
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="19">
+      <c r="C60" s="20">
         <v>64</v>
       </c>
     </row>
+    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B73" s="30"/>
+      <c r="C73" s="31"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C82" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C83" s="19">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A73:C73"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:B6"/>

</xml_diff>

<commit_message>
update web_form testing (Equivalent Class)
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Требования" sheetId="1" r:id="rId1"/>
-    <sheet name="Чек-листы" sheetId="2" r:id="rId2"/>
-    <sheet name="Тест-кейсы" sheetId="3" r:id="rId3"/>
-    <sheet name="Баг-репорты" sheetId="4" r:id="rId4"/>
-    <sheet name="Граничные значения" sheetId="5" r:id="rId5"/>
-    <sheet name="Классы эквивалентности" sheetId="6" r:id="rId6"/>
+    <sheet name="Классы эквивалентности" sheetId="6" r:id="rId2"/>
+    <sheet name="Чек-листы" sheetId="2" r:id="rId3"/>
+    <sheet name="Тест-кейсы" sheetId="3" r:id="rId4"/>
+    <sheet name="Баг-репорты" sheetId="4" r:id="rId5"/>
+    <sheet name="Граничные значения" sheetId="5" r:id="rId6"/>
     <sheet name="Попарное тестирование" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="233">
   <si>
     <t>ID</t>
   </si>
@@ -580,12 +580,237 @@
 1.В поле обязательно должны присутствовать: 1 буква в вернем регистре, 1 цифра, 1  @;
 2. Запрещено введение 2 и более  "@" подряд.</t>
   </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Windows 10 Home 19042.1706</t>
+  </si>
+  <si>
+    <t>Браузер</t>
+  </si>
+  <si>
+    <t>Chrome: 101.0.4951.67 (64 bit)</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>EN-1</t>
+  </si>
+  <si>
+    <t>Оставить поле Name Пустым</t>
+  </si>
+  <si>
+    <t>Ввести в поле Name валидное количество символов</t>
+  </si>
+  <si>
+    <t>EN-2</t>
+  </si>
+  <si>
+    <t>Name:
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Success Hello: Arina Strashchenko" и подсвечивается голубой тенью</t>
+  </si>
+  <si>
+    <t>Name: Arinaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Оставить поле Surname Пустым</t>
+  </si>
+  <si>
+    <t>Ввести в поле Surname валидное количество символов</t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Success Hello: Arina " и подсвечивается голубой тенью</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: 
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenkoooooooooooooooooooooooooooooooooooooooooooooooooooooo
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>ES-1</t>
+  </si>
+  <si>
+    <t>ES-2</t>
+  </si>
+  <si>
+    <t>EE-1</t>
+  </si>
+  <si>
+    <t>EE-2</t>
+  </si>
+  <si>
+    <t>ES-3</t>
+  </si>
+  <si>
+    <t>EN-3</t>
+  </si>
+  <si>
+    <t>EE-3</t>
+  </si>
+  <si>
+    <t>Оставить поле Email Пустым</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email валидное количество символов</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: @mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email:straschenko1333333333333333333333@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: 
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>EE-4</t>
+  </si>
+  <si>
+    <t>Ввести в поле Surname количество символов больше допустимого (&gt;64)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Name количество символов больше допустимого (&gt;64)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email до @ количество символов меньше допустимого (&lt;1)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email до @ количество символов больше допустимого (&gt;32)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после @ и до последней . количество символов меньше допустимого (&lt;2)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после @ и до последней .  количество символов больше допустимого (&gt;24)</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@m.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email:straschenko13@maillllllllllllllllllllll.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после последней .  количество символов меньше допустимого (&lt;2)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после последней .   количество символов больше допустимого (&gt;16)</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.r
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email:straschenko13@mail.ruuuuuuuuuuuuuuuu
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>EE-5</t>
+  </si>
+  <si>
+    <t>EE-6</t>
+  </si>
+  <si>
+    <t>EE-7</t>
+  </si>
+  <si>
+    <t>EE-8</t>
+  </si>
+  <si>
+    <t>Оставить поле Password Пустым</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password валидное количество символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password количество символов меньше допустимого (&lt;6)</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password количество символов больше допустимого (&gt;16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: </t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tD@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@588888888888</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +833,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -629,7 +862,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -796,12 +1029,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -812,21 +1084,28 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -860,9 +1139,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,26 +1172,52 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -970,6 +1272,43 @@
         <a:xfrm>
           <a:off x="9458324" y="257175"/>
           <a:ext cx="2743201" cy="2676525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>687104</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>37856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>845854</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>186022</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="64054" t="9170" r="35088" b="89423"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6240912" y="2338510"/>
+          <a:ext cx="158750" cy="148166"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1246,897 +1585,897 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:C83"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="74" style="24" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="74" style="25" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="20" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="20" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="20" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="20" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="20" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="20" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="20" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="20" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="21" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="36"/>
+      <c r="B39" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
+      <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="20" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="20" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="20" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="20" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="20" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="20">
         <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="36"/>
+      <c r="B50" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="16"/>
+      <c r="C50" s="17"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="19" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="19" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="20" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="20" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="20" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="20" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="19">
+      <c r="C59" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="20">
+      <c r="C60" s="21">
         <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="37"/>
+      <c r="B61" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="27"/>
       <c r="C61" s="28"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C63" s="19" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="20" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="20" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="20" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="20" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="20" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="20" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="38"/>
+      <c r="B73" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="B73" s="30"/>
-      <c r="C73" s="31"/>
+      <c r="C73" s="40"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="20" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="20" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="20" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="20" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="20" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C82" s="19">
+      <c r="C82" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C83" s="19">
+      <c r="C83" s="20">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A14:C14"/>
     <mergeCell ref="B16:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2147,13 +2486,515 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="31"/>
+    <col min="2" max="2" width="37.42578125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="31" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="31" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="9" max="11" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="29"/>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="29"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="29"/>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="29"/>
+    </row>
+    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="29"/>
+    </row>
+    <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A22:G22"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E10 E14 E23">
+      <formula1>"Passed,Failed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Требования!$A$3:$A$83</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6:F8 F10:F12 F14:F21 F23:F26</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update web_form testing (boundary)
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Требования" sheetId="1" r:id="rId1"/>
     <sheet name="Классы эквивалентности" sheetId="6" r:id="rId2"/>
-    <sheet name="Чек-листы" sheetId="2" r:id="rId3"/>
-    <sheet name="Тест-кейсы" sheetId="3" r:id="rId4"/>
-    <sheet name="Баг-репорты" sheetId="4" r:id="rId5"/>
-    <sheet name="Граничные значения" sheetId="5" r:id="rId6"/>
+    <sheet name="Граничные значения" sheetId="8" r:id="rId3"/>
+    <sheet name="Чек-листы" sheetId="2" r:id="rId4"/>
+    <sheet name="Тест-кейсы" sheetId="3" r:id="rId5"/>
+    <sheet name="Баг-репорты" sheetId="4" r:id="rId6"/>
     <sheet name="Попарное тестирование" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="299">
   <si>
     <t>ID</t>
   </si>
@@ -804,6 +804,246 @@
 Surname: Strashchenko
 Email: straschenko13@mail.ru
 Password: tDbb@588888888888</t>
+  </si>
+  <si>
+    <t>BN-1</t>
+  </si>
+  <si>
+    <t>BN-2</t>
+  </si>
+  <si>
+    <t>BN-3</t>
+  </si>
+  <si>
+    <t>BS-1</t>
+  </si>
+  <si>
+    <t>BS-2</t>
+  </si>
+  <si>
+    <t>BS-3</t>
+  </si>
+  <si>
+    <t>Ввести в поле Name 0 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Name 1 символ</t>
+  </si>
+  <si>
+    <t>Ввести в поле Name 64 символа</t>
+  </si>
+  <si>
+    <t>Ввести в поле Name 65 символов</t>
+  </si>
+  <si>
+    <t>Name: A
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arinaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>BN-4</t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Success Hello: A Strashchenko" и подсвечивается голубой тенью</t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Success Hello: Arinaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa Strashchenko" и подсвечивается голубой тенью</t>
+  </si>
+  <si>
+    <t>BS-4</t>
+  </si>
+  <si>
+    <t>Ввести в поле Surname 0 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Surname 1 символ</t>
+  </si>
+  <si>
+    <t>Ввести в поле Surname 64 символа</t>
+  </si>
+  <si>
+    <t>Ввести в поле Surname 65 символов</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: S
+Email: straschenko13@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Success Hello: Arina S" и подсвечивается голубой тенью</t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Success Hello: Arina Strashchenkoooooooooooooooooooooooooooooooooooooooooooooooooooooo" и подсвечивается голубой тенью</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password 5 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password 6 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password 17 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Password 16 символов</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDb@5</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@5</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@58888888888</t>
+  </si>
+  <si>
+    <t>BP-1</t>
+  </si>
+  <si>
+    <t>BP-2</t>
+  </si>
+  <si>
+    <t>BP-3</t>
+  </si>
+  <si>
+    <t>BP-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поле Email  0 символов до @ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поле Email  1 символ до @ </t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: s@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поле Email  32 символа до @ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поле Email  33 символа до @ </t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после @ и до последней .  1 символ</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после @ и до последней .  2 символа</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после @ и до последней .  24 символа</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после @ и до последней .  25 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после последней .  1 символ</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после последней .  2 символа</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после последней .  16 символов</t>
+  </si>
+  <si>
+    <t>Ввести в поле Email после последней .  17 символов</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko133333333333333333333@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko1333333333333333333333@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@m.rг
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@ma.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mailllllllllllllllllllll.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ruuuuuuuuuuuuuuu
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email: straschenko13@mail.ruuuuuuuuuuuuuuuu
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>BE-3</t>
+  </si>
+  <si>
+    <t>BE-7</t>
+  </si>
+  <si>
+    <t>BE-1</t>
+  </si>
+  <si>
+    <t>BE-2</t>
+  </si>
+  <si>
+    <t>BE-4</t>
+  </si>
+  <si>
+    <t>BE-5</t>
+  </si>
+  <si>
+    <t>BE-6</t>
+  </si>
+  <si>
+    <t>BE-8</t>
+  </si>
+  <si>
+    <t>BE-9</t>
+  </si>
+  <si>
+    <t>BE-10</t>
+  </si>
+  <si>
+    <t>BE-11</t>
+  </si>
+  <si>
+    <t>BE-12</t>
   </si>
 </sst>
 </file>
@@ -1121,30 +1361,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1163,20 +1379,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1186,15 +1393,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1206,14 +1404,56 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1585,32 +1825,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="74" style="25" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="74" style="16" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1618,10 +1858,10 @@
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1629,8 +1869,8 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1638,8 +1878,8 @@
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1647,8 +1887,8 @@
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1656,10 +1896,10 @@
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1667,8 +1907,8 @@
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1676,8 +1916,8 @@
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1688,7 +1928,7 @@
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1699,7 +1939,7 @@
       <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1710,7 +1950,7 @@
       <c r="B12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1721,16 +1961,16 @@
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="27"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -1739,7 +1979,7 @@
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1747,10 +1987,10 @@
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1758,8 +1998,8 @@
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="20" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1767,8 +2007,8 @@
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="20" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1776,10 +2016,10 @@
       <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="12" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1787,8 +2027,8 @@
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1796,8 +2036,8 @@
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="20" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="12" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1805,8 +2045,8 @@
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="20" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="12" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1817,7 +2057,7 @@
       <c r="B23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="12" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1828,7 +2068,7 @@
       <c r="B24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="12" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1839,7 +2079,7 @@
       <c r="B25" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="12" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1850,7 +2090,7 @@
       <c r="B26" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1861,7 +2101,7 @@
       <c r="B27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1872,7 +2112,7 @@
       <c r="B28" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1883,7 +2123,7 @@
       <c r="B29" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="12" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1894,7 +2134,7 @@
       <c r="B30" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="12" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1905,7 +2145,7 @@
       <c r="B31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="12" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1916,7 +2156,7 @@
       <c r="B32" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="12" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1927,7 +2167,7 @@
       <c r="B33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1938,7 +2178,7 @@
       <c r="B34" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="12" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1949,7 +2189,7 @@
       <c r="B35" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="12" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1960,7 +2200,7 @@
       <c r="B36" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="12" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1971,7 +2211,7 @@
       <c r="B37" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="12" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1982,16 +2222,16 @@
       <c r="B38" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
-      <c r="B39" s="16" t="s">
+      <c r="A39" s="22"/>
+      <c r="B39" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="27"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
@@ -2000,7 +2240,7 @@
       <c r="B40" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2011,7 +2251,7 @@
       <c r="B41" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="12" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2022,7 +2262,7 @@
       <c r="B42" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2033,7 +2273,7 @@
       <c r="B43" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2044,7 +2284,7 @@
       <c r="B44" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="12" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2055,7 +2295,7 @@
       <c r="B45" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="12" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2066,7 +2306,7 @@
       <c r="B46" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="12" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2077,7 +2317,7 @@
       <c r="B47" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="12" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2088,7 +2328,7 @@
       <c r="B48" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="20">
+      <c r="C48" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2099,16 +2339,16 @@
       <c r="B49" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C49" s="12">
         <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="16" t="s">
+      <c r="A50" s="22"/>
+      <c r="B50" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="17"/>
+      <c r="C50" s="27"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
@@ -2117,7 +2357,7 @@
       <c r="B51" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2128,7 +2368,7 @@
       <c r="B52" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2139,7 +2379,7 @@
       <c r="B53" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2150,7 +2390,7 @@
       <c r="B54" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2161,7 +2401,7 @@
       <c r="B55" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="12" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2172,7 +2412,7 @@
       <c r="B56" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="12" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2183,7 +2423,7 @@
       <c r="B57" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="12" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2194,7 +2434,7 @@
       <c r="B58" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="12" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2205,7 +2445,7 @@
       <c r="B59" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="20">
+      <c r="C59" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2216,16 +2456,16 @@
       <c r="B60" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="21">
+      <c r="C60" s="13">
         <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="37"/>
-      <c r="B61" s="27" t="s">
+      <c r="A61" s="23"/>
+      <c r="B61" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="28"/>
+      <c r="C61" s="29"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
@@ -2234,7 +2474,7 @@
       <c r="B62" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2245,7 +2485,7 @@
       <c r="B63" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2256,7 +2496,7 @@
       <c r="B64" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2267,7 +2507,7 @@
       <c r="B65" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2278,7 +2518,7 @@
       <c r="B66" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="12" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2289,7 +2529,7 @@
       <c r="B67" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2300,7 +2540,7 @@
       <c r="B68" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="12" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2311,7 +2551,7 @@
       <c r="B69" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="12" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2322,7 +2562,7 @@
       <c r="B70" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="12" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2333,7 +2573,7 @@
       <c r="B71" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="12" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2344,16 +2584,16 @@
       <c r="B72" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="12" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="38"/>
-      <c r="B73" s="39" t="s">
+      <c r="A73" s="24"/>
+      <c r="B73" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="C73" s="40"/>
+      <c r="C73" s="31"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
@@ -2362,7 +2602,7 @@
       <c r="B74" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2373,7 +2613,7 @@
       <c r="B75" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="12" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2384,7 +2624,7 @@
       <c r="B76" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2395,7 +2635,7 @@
       <c r="B77" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2406,7 +2646,7 @@
       <c r="B78" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="12" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2417,7 +2657,7 @@
       <c r="B79" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="12" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2428,7 +2668,7 @@
       <c r="B80" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C80" s="12" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2439,7 +2679,7 @@
       <c r="B81" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="C81" s="12" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2450,7 +2690,7 @@
       <c r="B82" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C82" s="20">
+      <c r="C82" s="12">
         <v>6</v>
       </c>
     </row>
@@ -2461,22 +2701,22 @@
       <c r="B83" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C83" s="20">
+      <c r="C83" s="12">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B16:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2488,486 +2728,486 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="31"/>
-    <col min="2" max="2" width="37.42578125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="31" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="31" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="31" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="2" max="2" width="37.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="20" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="4"/>
     <col min="9" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="19" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="19" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="19" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
     </row>
     <row r="6" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F7" s="29" t="s">
+      <c r="E7" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" s="29" t="s">
+      <c r="E8" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="29"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="29" t="s">
+      <c r="E10" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="29"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F11" s="29" t="s">
+      <c r="E11" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="29"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F12" s="29" t="s">
+      <c r="E12" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F14" s="29" t="s">
+      <c r="E14" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F15" s="29" t="s">
+      <c r="E15" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F16" s="29" t="s">
+      <c r="E16" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F17" s="29" t="s">
+      <c r="E17" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F18" s="29" t="s">
+      <c r="E18" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="29"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F19" s="29" t="s">
+      <c r="E19" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="29"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" s="29" t="s">
+      <c r="E20" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F21" s="29" t="s">
+      <c r="E21" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="29"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="34"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F23" s="29" t="s">
+      <c r="E23" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="29"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F24" s="29" t="s">
+      <c r="E24" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="29"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F25" s="29" t="s">
+      <c r="E25" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="29"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F26" s="29" t="s">
+      <c r="E26" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="29"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="41"/>
+      <c r="C27" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3000,13 +3240,728 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="2" max="2" width="37.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="4" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+    </row>
+    <row r="6" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="18"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A28:G28"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E11:E14 E29">
+      <formula1>"Passed,Failed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Требования!$A$3:$A$83</xm:f>
+          </x14:formula1>
+          <xm:sqref>F29:F32 F6:F9 F11:F14 F16:F27</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update web_form testing (check lists)
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Требования" sheetId="1" r:id="rId1"/>
     <sheet name="Классы эквивалентности" sheetId="6" r:id="rId2"/>
     <sheet name="Граничные значения" sheetId="8" r:id="rId3"/>
-    <sheet name="Чек-листы" sheetId="2" r:id="rId4"/>
-    <sheet name="Тест-кейсы" sheetId="3" r:id="rId5"/>
-    <sheet name="Баг-репорты" sheetId="4" r:id="rId6"/>
-    <sheet name="Попарное тестирование" sheetId="7" r:id="rId7"/>
+    <sheet name="Попарное тестирование" sheetId="7" r:id="rId4"/>
+    <sheet name="Чек-листы" sheetId="9" r:id="rId5"/>
+    <sheet name="Тест-кейсы" sheetId="3" r:id="rId6"/>
+    <sheet name="Баг-репорты" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="330">
   <si>
     <t>ID</t>
   </si>
@@ -884,6 +884,9 @@
     <t>Под кнопкой "Submit" отображается сообщение "Success Hello: Arina Strashchenkoooooooooooooooooooooooooooooooooooooooooooooooooooooo" и подсвечивается голубой тенью</t>
   </si>
   <si>
+    <t>Ввести в поле Password 0 символов</t>
+  </si>
+  <si>
     <t>Ввести в поле Password 5 символов</t>
   </si>
   <si>
@@ -1044,13 +1047,172 @@
   </si>
   <si>
     <t>BE-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поле Email  0 символов  </t>
+  </si>
+  <si>
+    <t>валидное</t>
+  </si>
+  <si>
+    <t>невалидное</t>
+  </si>
+  <si>
+    <t>пустое</t>
+  </si>
+  <si>
+    <t>PF-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - валидное значение
+Surname - валидное значение
+Email - валидное значение
+Password - валидное значение
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - валидное значение
+Surname - невалидное значение
+Email - невалидное значение
+Password - невалидное значение
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - валидное значение
+Surname - валидное значение
+Email - пустое
+Password - пустое
+</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenko
+Email:
+Password:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - невалидное значение
+Surname - валидное значение
+Email - невалидное значение
+Password - пустое
+</t>
+  </si>
+  <si>
+    <t>Name: Arina
+Surname: Strashchenkoo?
+Email: straschenko13@mail.ru#
+Password:  tDb@5%</t>
+  </si>
+  <si>
+    <t>Name: Arina&gt;
+Surname: Strashchenko
+Email: straschenko13@mail.ru!
+Password:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name -  невалидное значение
+Surname - невалидное значение
+Email - пустое
+Password - валидное значение
+</t>
+  </si>
+  <si>
+    <t>Name: Arina$
+Surname: Strashchenko^
+Email:
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - невалидное значение
+Surname - валидное значение
+Email - валидное значение
+Password - невалидное значение
+</t>
+  </si>
+  <si>
+    <t>Name: Arina+
+Surname: Strashchenko
+Email: straschenko13@mail.ru
+Password: tDbb@@58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name -  пустое
+Surname - валидное значение
+Email - пустое
+Password - невалидное значение
+</t>
+  </si>
+  <si>
+    <t>Name: 
+Surname: Strashchenko
+Email: 
+Password: tDbb@58.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - пустое
+Surname - невалидное значение
+Email - валидное значение
+Password - пустое
+</t>
+  </si>
+  <si>
+    <t>Name: 
+Surname: Strashchenko//
+Email: straschenko13@mail.ru
+Password:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поля:
+Name - пустое
+Surname - валидное значение
+Email - невалидное значение
+Password - валидное значение
+</t>
+  </si>
+  <si>
+    <t>Name: 
+Surname: Strashchenko
+Email: straschenko13@@mail.ru
+Password: tDbb@58</t>
+  </si>
+  <si>
+    <t>PF-2</t>
+  </si>
+  <si>
+    <t>PF-3</t>
+  </si>
+  <si>
+    <t>PF-4</t>
+  </si>
+  <si>
+    <t>PF-5</t>
+  </si>
+  <si>
+    <t>PF-6</t>
+  </si>
+  <si>
+    <t>PF-7</t>
+  </si>
+  <si>
+    <t>PF-8</t>
+  </si>
+  <si>
+    <t>PF-9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1081,8 +1243,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1098,6 +1272,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0D0FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1330,11 +1528,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1455,19 +1654,55 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FF00FF00"/>
       <color rgb="FFE0D0FC"/>
       <color rgb="FFDCC5FB"/>
       <color rgb="FFE2B2F8"/>
-      <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1825,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -2728,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,9 +3477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3528,10 +3761,10 @@
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>206</v>
@@ -3552,13 +3785,13 @@
     </row>
     <row r="17" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>194</v>
@@ -3576,13 +3809,13 @@
     </row>
     <row r="18" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>194</v>
@@ -3600,13 +3833,13 @@
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>54</v>
@@ -3624,13 +3857,13 @@
     </row>
     <row r="20" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>54</v>
@@ -3648,13 +3881,13 @@
     </row>
     <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>194</v>
@@ -3672,13 +3905,13 @@
     </row>
     <row r="22" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>194</v>
@@ -3696,13 +3929,13 @@
     </row>
     <row r="23" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>54</v>
@@ -3720,10 +3953,10 @@
     </row>
     <row r="24" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>220</v>
@@ -3744,10 +3977,10 @@
     </row>
     <row r="25" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>189</v>
@@ -3768,13 +4001,13 @@
     </row>
     <row r="26" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>194</v>
@@ -3792,13 +4025,13 @@
     </row>
     <row r="27" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>54</v>
@@ -3830,13 +4063,13 @@
     </row>
     <row r="29" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>54</v>
@@ -3854,13 +4087,13 @@
     </row>
     <row r="30" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>190</v>
@@ -3878,13 +4111,13 @@
     </row>
     <row r="31" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>190</v>
@@ -3902,10 +4135,10 @@
     </row>
     <row r="32" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>232</v>
@@ -3967,25 +4200,1108 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="12.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="2" max="2" width="37.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="4" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="49"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="49"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="50"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="50"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="53"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="50"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="50"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="50"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="53"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="53"/>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="50"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="50"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>292</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="53"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
+        <v>293</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="53"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="50" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>284</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="50"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>275</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>276</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>285</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="53"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="53"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="50"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="53"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="53"/>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="53"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="50"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>263</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="E29" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>259</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="53"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
+        <v>304</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>305</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
+        <v>322</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>306</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>310</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="53"/>
+    </row>
+    <row r="33" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>308</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="53"/>
+    </row>
+    <row r="34" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>311</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="53"/>
+    </row>
+    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>312</v>
+      </c>
+      <c r="C35" s="53" t="s">
+        <v>313</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="53"/>
+    </row>
+    <row r="36" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>314</v>
+      </c>
+      <c r="C36" s="53" t="s">
+        <v>315</v>
+      </c>
+      <c r="D36" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" s="53"/>
+    </row>
+    <row r="37" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="B37" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="C37" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="D37" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37" s="53"/>
+    </row>
+    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="B38" s="53" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="53" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" s="53"/>
+    </row>
+    <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>320</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>321</v>
+      </c>
+      <c r="D39" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="53"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E26:E27 E9:E13">
+      <formula1>"Passed,Failed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Требования!$A$3:$A$83</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5:F39</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update web form testing Postman
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Требования" sheetId="1" r:id="rId1"/>
@@ -2623,7 +2623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -3548,8 +3548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5701,7 +5701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -7041,7 +7041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update web form testing (test cases)
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Требования" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="465">
   <si>
     <t>ID</t>
   </si>
@@ -1622,6 +1622,9 @@
   </si>
   <si>
     <t xml:space="preserve">Нажатие кнопки "Обновить" </t>
+  </si>
+  <si>
+    <t>Под кнопкой "Submit" отображается сообщение "Error: Error: All Fields are Required" и подсвечивается красной тенью</t>
   </si>
 </sst>
 </file>
@@ -2065,54 +2068,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2162,6 +2117,54 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2621,10 +2624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,11 +2638,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -2656,7 +2659,7 @@
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="68" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -2667,7 +2670,7 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="44"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
@@ -2676,7 +2679,7 @@
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="44"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
@@ -2685,7 +2688,7 @@
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="45"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
@@ -2694,7 +2697,7 @@
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="71" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -2705,7 +2708,7 @@
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="44"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
@@ -2714,7 +2717,7 @@
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="45"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
@@ -2765,10 +2768,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="48"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -2785,7 +2788,7 @@
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="71" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -2796,7 +2799,7 @@
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="44"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="12" t="s">
         <v>34</v>
       </c>
@@ -2805,7 +2808,7 @@
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="45"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="12" t="s">
         <v>35</v>
       </c>
@@ -2814,7 +2817,7 @@
       <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="65" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -2825,7 +2828,7 @@
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="53"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="12" t="s">
         <v>43</v>
       </c>
@@ -2834,7 +2837,7 @@
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="53"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="12" t="s">
         <v>92</v>
       </c>
@@ -2843,7 +2846,7 @@
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="53"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="12" t="s">
         <v>93</v>
       </c>
@@ -2998,7 +3001,7 @@
       <c r="B36" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="56" t="s">
         <v>416</v>
       </c>
     </row>
@@ -3048,10 +3051,10 @@
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="48"/>
+      <c r="C41" s="60"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -3165,10 +3168,10 @@
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22"/>
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="48"/>
+      <c r="C52" s="60"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
@@ -3282,10 +3285,10 @@
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="23"/>
-      <c r="B63" s="49" t="s">
+      <c r="B63" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="50"/>
+      <c r="C63" s="62"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
@@ -3298,7 +3301,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>131</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>132</v>
       </c>
@@ -3320,7 +3323,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>133</v>
       </c>
@@ -3331,7 +3334,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>134</v>
       </c>
@@ -3342,7 +3345,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>135</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>136</v>
       </c>
@@ -3364,7 +3367,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>137</v>
       </c>
@@ -3375,7 +3378,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>138</v>
       </c>
@@ -3386,7 +3389,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>146</v>
       </c>
@@ -3396,8 +3399,17 @@
       <c r="C73" s="12" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>32</v>
+      </c>
+      <c r="E73">
+        <v>24</v>
+      </c>
+      <c r="F73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>149</v>
       </c>
@@ -3408,14 +3420,14 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="24"/>
-      <c r="B75" s="51" t="s">
+      <c r="B75" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="C75" s="52"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="64"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>154</v>
       </c>
@@ -3426,7 +3438,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>155</v>
       </c>
@@ -3437,7 +3449,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>156</v>
       </c>
@@ -3448,7 +3460,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>157</v>
       </c>
@@ -3459,7 +3471,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>158</v>
       </c>
@@ -3527,16 +3539,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3548,22 +3560,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:XFD76"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="20"/>
     <col min="2" max="2" width="37.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="70" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="54" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" style="14" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="20" customWidth="1"/>
     <col min="6" max="6" width="31.5703125" style="20" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" style="20" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" style="20" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="4" customWidth="1"/>
     <col min="11" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -3574,7 +3586,7 @@
       <c r="B1" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="66"/>
+      <c r="C1" s="50"/>
       <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3584,7 +3596,7 @@
       <c r="B2" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="66"/>
+      <c r="C2" s="50"/>
       <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3594,10 +3606,10 @@
       <c r="B4" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="51" t="s">
         <v>387</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="57" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="19" t="s">
@@ -3616,1032 +3628,1032 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+    <row r="5" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="58" t="s">
+      <c r="D5" s="44"/>
+      <c r="E5" s="42" t="s">
         <v>390</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-    </row>
-    <row r="6" spans="1:13" s="63" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="I5" s="42"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+    </row>
+    <row r="6" spans="1:13" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
         <v>330</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="42" t="s">
         <v>329</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D6" s="60"/>
-      <c r="E6" s="58" t="s">
+      <c r="D6" s="44"/>
+      <c r="E6" s="42" t="s">
         <v>390</v>
       </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="57" t="s">
+      <c r="F6" s="42"/>
+      <c r="G6" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-    </row>
-    <row r="7" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="I6" s="42"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+    </row>
+    <row r="7" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="58" t="s">
+      <c r="D7" s="44"/>
+      <c r="E7" s="42" t="s">
         <v>391</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H7" s="58" t="s">
+      <c r="H7" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-    </row>
-    <row r="8" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="I7" s="42"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+    </row>
+    <row r="8" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
         <v>345</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="42" t="s">
         <v>349</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="58" t="s">
+      <c r="D8" s="44"/>
+      <c r="E8" s="42" t="s">
         <v>392</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="42" t="s">
         <v>353</v>
       </c>
-      <c r="G8" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-    </row>
-    <row r="9" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="G8" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+    </row>
+    <row r="9" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
         <v>346</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="42" t="s">
         <v>350</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="58" t="s">
+      <c r="D9" s="44"/>
+      <c r="E9" s="42" t="s">
         <v>393</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="G9" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-    </row>
-    <row r="10" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="G9" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+    </row>
+    <row r="10" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="58" t="s">
+      <c r="D10" s="44"/>
+      <c r="E10" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="42" t="s">
         <v>355</v>
       </c>
-      <c r="G10" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-    </row>
-    <row r="11" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="G10" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+    </row>
+    <row r="11" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
         <v>348</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="44"/>
+      <c r="E11" s="42" t="s">
         <v>395</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="42" t="s">
         <v>356</v>
       </c>
-      <c r="G11" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-    </row>
-    <row r="12" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="G11" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+    </row>
+    <row r="12" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="42" t="s">
         <v>341</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="58" t="s">
+      <c r="D12" s="44"/>
+      <c r="E12" s="42" t="s">
         <v>396</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-    </row>
-    <row r="13" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+    </row>
+    <row r="13" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
         <v>338</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="42" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="58" t="s">
+      <c r="D13" s="44"/>
+      <c r="E13" s="42" t="s">
         <v>397</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="42" t="s">
         <v>335</v>
       </c>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-    </row>
-    <row r="14" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+    </row>
+    <row r="14" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
         <v>339</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="42" t="s">
         <v>343</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="58" t="s">
+      <c r="D14" s="44"/>
+      <c r="E14" s="42" t="s">
         <v>398</v>
       </c>
-      <c r="F14" s="58" t="s">
+      <c r="F14" s="42" t="s">
         <v>336</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-    </row>
-    <row r="15" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+    </row>
+    <row r="15" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
         <v>340</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="42" t="s">
         <v>344</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="58" t="s">
+      <c r="D15" s="44"/>
+      <c r="E15" s="42" t="s">
         <v>399</v>
       </c>
-      <c r="F15" s="58" t="s">
+      <c r="F15" s="42" t="s">
         <v>337</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-    </row>
-    <row r="16" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+    </row>
+    <row r="16" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
         <v>365</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D16" s="60"/>
-      <c r="E16" s="58" t="s">
+      <c r="D16" s="44"/>
+      <c r="E16" s="42" t="s">
         <v>400</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F16" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="57" t="s">
+      <c r="G16" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-    </row>
-    <row r="17" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="58" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+    </row>
+    <row r="17" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
         <v>366</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="58" t="s">
+      <c r="D17" s="44"/>
+      <c r="E17" s="42" t="s">
         <v>401</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="57" t="s">
+      <c r="G17" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-    </row>
-    <row r="18" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+    </row>
+    <row r="18" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
         <v>367</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="42" t="s">
         <v>359</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="58" t="s">
+      <c r="D18" s="44"/>
+      <c r="E18" s="42" t="s">
         <v>402</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="57" t="s">
+      <c r="G18" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="62"/>
-    </row>
-    <row r="19" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+    </row>
+    <row r="19" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
         <v>368</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="42" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="58" t="s">
+      <c r="D19" s="44"/>
+      <c r="E19" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-    </row>
-    <row r="20" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+    </row>
+    <row r="20" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
         <v>372</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="58" t="s">
+      <c r="D20" s="44"/>
+      <c r="E20" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="G20" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-    </row>
-    <row r="21" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+      <c r="G20" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+    </row>
+    <row r="21" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
         <v>373</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="42" t="s">
         <v>362</v>
       </c>
-      <c r="C21" s="68" t="s">
+      <c r="C21" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="58" t="s">
+      <c r="D21" s="44"/>
+      <c r="E21" s="42" t="s">
         <v>406</v>
       </c>
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="G21" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="62"/>
-    </row>
-    <row r="22" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="G21" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+    </row>
+    <row r="22" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>374</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="42" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="58" t="s">
+      <c r="D22" s="44"/>
+      <c r="E22" s="42" t="s">
         <v>407</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="G22" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="62"/>
-    </row>
-    <row r="23" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
+      <c r="G22" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+    </row>
+    <row r="23" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
         <v>375</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="42" t="s">
         <v>364</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="58" t="s">
+      <c r="D23" s="44"/>
+      <c r="E23" s="42" t="s">
         <v>408</v>
       </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="G23" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-    </row>
-    <row r="24" spans="1:13" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="G23" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+    </row>
+    <row r="24" spans="1:13" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="42" t="s">
         <v>420</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>419</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="44" t="s">
         <v>431</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="42" t="s">
         <v>427</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
-    </row>
-    <row r="25" spans="1:13" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
+      <c r="G24" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+    </row>
+    <row r="25" spans="1:13" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
         <v>421</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="C25" s="68" t="s">
+      <c r="C25" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="44" t="s">
         <v>432</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="42" t="s">
         <v>428</v>
       </c>
-      <c r="F25" s="60" t="s">
+      <c r="F25" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
-    </row>
-    <row r="26" spans="1:13" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="G25" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+    </row>
+    <row r="26" spans="1:13" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
         <v>422</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="44" t="s">
         <v>433</v>
       </c>
-      <c r="E26" s="58" t="s">
+      <c r="E26" s="42" t="s">
         <v>429</v>
       </c>
-      <c r="F26" s="60" t="s">
+      <c r="F26" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-    </row>
-    <row r="27" spans="1:13" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
+      <c r="G26" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+    </row>
+    <row r="27" spans="1:13" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="42" t="s">
         <v>423</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="C27" s="68" t="s">
+      <c r="C27" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="44">
         <v>111111</v>
       </c>
-      <c r="E27" s="58" t="s">
+      <c r="E27" s="42" t="s">
         <v>430</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-    </row>
-    <row r="28" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
+      <c r="G27" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+    </row>
+    <row r="28" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="42" t="s">
         <v>438</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="44" t="s">
         <v>446</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="42" t="s">
         <v>443</v>
       </c>
-      <c r="F28" s="60" t="s">
+      <c r="F28" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="57" t="s">
+      <c r="G28" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-    </row>
-    <row r="29" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+    </row>
+    <row r="29" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
         <v>439</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>435</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="44" t="s">
         <v>447</v>
       </c>
-      <c r="E29" s="58" t="s">
+      <c r="E29" s="42" t="s">
         <v>444</v>
       </c>
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G29" s="57" t="s">
+      <c r="G29" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-    </row>
-    <row r="30" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+    </row>
+    <row r="30" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="42" t="s">
         <v>440</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>436</v>
       </c>
-      <c r="C30" s="68" t="s">
+      <c r="C30" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D30" s="74" t="s">
+      <c r="D30" s="58" t="s">
         <v>448</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="42" t="s">
         <v>445</v>
       </c>
-      <c r="F30" s="60" t="s">
+      <c r="F30" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-    </row>
-    <row r="31" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+    </row>
+    <row r="31" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
         <v>441</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="C31" s="68" t="s">
+      <c r="C31" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D31" s="74" t="s">
+      <c r="D31" s="58" t="s">
         <v>449</v>
       </c>
-      <c r="E31" s="58" t="s">
+      <c r="E31" s="42" t="s">
         <v>442</v>
       </c>
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="57" t="s">
+      <c r="G31" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
-    </row>
-    <row r="32" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="58" t="s">
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+    </row>
+    <row r="32" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="42" t="s">
         <v>454</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="C32" s="68" t="s">
+      <c r="C32" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="44" t="s">
         <v>458</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="42" t="s">
         <v>462</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="57" t="s">
+      <c r="G32" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="62"/>
-      <c r="M32" s="62"/>
-    </row>
-    <row r="33" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="58" t="s">
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+    </row>
+    <row r="33" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
         <v>455</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="C33" s="68" t="s">
+      <c r="C33" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="44" t="s">
         <v>459</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="42" t="s">
         <v>462</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G33" s="57" t="s">
+      <c r="G33" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-    </row>
-    <row r="34" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+    </row>
+    <row r="34" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
         <v>456</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="C34" s="68" t="s">
+      <c r="C34" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D34" s="74" t="s">
+      <c r="D34" s="58" t="s">
         <v>460</v>
       </c>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="42" t="s">
         <v>462</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G34" s="57" t="s">
+      <c r="G34" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
-      <c r="M34" s="62"/>
-    </row>
-    <row r="35" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+    </row>
+    <row r="35" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
         <v>457</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="C35" s="68" t="s">
+      <c r="C35" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D35" s="74" t="s">
+      <c r="D35" s="58" t="s">
         <v>461</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="42" t="s">
         <v>462</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G35" s="57" t="s">
+      <c r="G35" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="62"/>
-    </row>
-    <row r="36" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+    </row>
+    <row r="36" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
         <v>379</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="42" t="s">
         <v>376</v>
       </c>
-      <c r="C36" s="68" t="s">
+      <c r="C36" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D36" s="60"/>
-      <c r="E36" s="58" t="s">
+      <c r="D36" s="44"/>
+      <c r="E36" s="42" t="s">
         <v>409</v>
       </c>
-      <c r="F36" s="60" t="s">
+      <c r="F36" s="44" t="s">
         <v>378</v>
       </c>
-      <c r="G36" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="62"/>
-      <c r="M36" s="62"/>
-    </row>
-    <row r="37" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="G36" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+    </row>
+    <row r="37" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="42" t="s">
         <v>377</v>
       </c>
-      <c r="C37" s="68" t="s">
+      <c r="C37" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D37" s="60"/>
-      <c r="E37" s="58" t="s">
+      <c r="D37" s="44"/>
+      <c r="E37" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="F37" s="60" t="s">
+      <c r="F37" s="44" t="s">
         <v>378</v>
       </c>
-      <c r="G37" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="62"/>
-      <c r="M37" s="62"/>
-    </row>
-    <row r="38" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="G37" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+    </row>
+    <row r="38" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="42" t="s">
         <v>383</v>
       </c>
-      <c r="C38" s="68" t="s">
+      <c r="C38" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="58" t="s">
+      <c r="D38" s="44"/>
+      <c r="E38" s="42" t="s">
         <v>404</v>
       </c>
-      <c r="F38" s="60" t="s">
+      <c r="F38" s="44" t="s">
         <v>386</v>
       </c>
-      <c r="G38" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="62"/>
-      <c r="L38" s="62"/>
-      <c r="M38" s="62"/>
-    </row>
-    <row r="39" spans="1:13" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="58" t="s">
+      <c r="G38" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+    </row>
+    <row r="39" spans="1:13" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="42" t="s">
         <v>385</v>
       </c>
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="48" t="s">
         <v>381</v>
       </c>
-      <c r="C39" s="68" t="s">
+      <c r="C39" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="58" t="s">
+      <c r="D39" s="44"/>
+      <c r="E39" s="42" t="s">
         <v>410</v>
       </c>
-      <c r="F39" s="60" t="s">
+      <c r="F39" s="44" t="s">
         <v>415</v>
       </c>
-      <c r="G39" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="62"/>
-      <c r="L39" s="62"/>
-      <c r="M39" s="62"/>
-    </row>
-    <row r="40" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="58" t="s">
+      <c r="G39" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+    </row>
+    <row r="40" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="42" t="s">
         <v>385</v>
       </c>
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="48" t="s">
         <v>414</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="58" t="s">
+      <c r="D40" s="44"/>
+      <c r="E40" s="42" t="s">
         <v>410</v>
       </c>
-      <c r="F40" s="60" t="s">
+      <c r="F40" s="44" t="s">
         <v>416</v>
       </c>
-      <c r="G40" s="57" t="s">
+      <c r="G40" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="61"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="62"/>
-      <c r="M40" s="62"/>
-    </row>
-    <row r="41" spans="1:13" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="58" t="s">
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+    </row>
+    <row r="41" spans="1:13" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="42" t="s">
         <v>413</v>
       </c>
-      <c r="B41" s="64" t="s">
+      <c r="B41" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="52" t="s">
         <v>389</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="58" t="s">
+      <c r="D41" s="44"/>
+      <c r="E41" s="42" t="s">
         <v>411</v>
       </c>
-      <c r="F41" s="58" t="s">
+      <c r="F41" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="57" t="s">
+      <c r="G41" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="62"/>
-      <c r="M41" s="62"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
     </row>
     <row r="42" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="38" t="s">
@@ -4650,7 +4662,7 @@
       <c r="B42" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="C42" s="69" t="s">
+      <c r="C42" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D42" s="40" t="s">
@@ -4662,7 +4674,7 @@
       <c r="F42" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="39" t="s">
+      <c r="G42" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H42" s="38" t="s">
@@ -4677,7 +4689,7 @@
       <c r="B43" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D43" s="36" t="s">
@@ -4689,13 +4701,16 @@
       <c r="F43" s="36" t="s">
         <v>241</v>
       </c>
-      <c r="G43" s="37" t="s">
-        <v>183</v>
+      <c r="G43" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H43" s="35" t="s">
         <v>75</v>
       </c>
       <c r="I43" s="35"/>
+      <c r="J43" s="38" t="s">
+        <v>51</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -4707,7 +4722,7 @@
       <c r="B44" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D44" s="36" t="s">
@@ -4719,8 +4734,8 @@
       <c r="F44" s="36" t="s">
         <v>242</v>
       </c>
-      <c r="G44" s="37" t="s">
-        <v>183</v>
+      <c r="G44" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H44" s="35" t="s">
         <v>75</v>
@@ -4737,7 +4752,7 @@
       <c r="B45" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D45" s="40" t="s">
@@ -4749,7 +4764,7 @@
       <c r="F45" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G45" s="39" t="s">
+      <c r="G45" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H45" s="38" t="s">
@@ -4767,7 +4782,7 @@
       <c r="B46" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="C46" s="69" t="s">
+      <c r="C46" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D46" s="36" t="s">
@@ -4779,13 +4794,16 @@
       <c r="F46" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G46" s="37" t="s">
-        <v>183</v>
+      <c r="G46" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H46" s="35" t="s">
         <v>76</v>
       </c>
       <c r="I46" s="35"/>
+      <c r="J46" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -4797,7 +4815,7 @@
       <c r="B47" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="C47" s="69" t="s">
+      <c r="C47" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D47" s="36" t="s">
@@ -4809,7 +4827,7 @@
       <c r="F47" s="36" t="s">
         <v>249</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="G47" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H47" s="35" t="s">
@@ -4827,7 +4845,7 @@
       <c r="B48" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="C48" s="69" t="s">
+      <c r="C48" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D48" s="36" t="s">
@@ -4839,7 +4857,7 @@
       <c r="F48" s="36" t="s">
         <v>250</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="G48" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H48" s="35" t="s">
@@ -4857,7 +4875,7 @@
       <c r="B49" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="C49" s="69" t="s">
+      <c r="C49" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D49" s="40" t="s">
@@ -4869,25 +4887,28 @@
       <c r="F49" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G49" s="39" t="s">
-        <v>183</v>
+      <c r="G49" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H49" s="38" t="s">
         <v>77</v>
       </c>
       <c r="I49" s="38"/>
+      <c r="J49" s="36" t="s">
+        <v>250</v>
+      </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="38" t="s">
         <v>194</v>
       </c>
       <c r="B50" s="38" t="s">
         <v>295</v>
       </c>
-      <c r="C50" s="69" t="s">
+      <c r="C50" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D50" s="40" t="s">
@@ -4899,22 +4920,25 @@
       <c r="F50" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G50" s="39" t="s">
-        <v>183</v>
+      <c r="G50" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H50" s="38" t="s">
         <v>76</v>
       </c>
       <c r="I50" s="38"/>
-    </row>
-    <row r="51" spans="1:13" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="J50" s="36" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
         <v>285</v>
       </c>
       <c r="B51" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="C51" s="69" t="s">
+      <c r="C51" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D51" s="40" t="s">
@@ -4926,13 +4950,16 @@
       <c r="F51" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G51" s="39" t="s">
-        <v>183</v>
+      <c r="G51" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H51" s="38" t="s">
         <v>77</v>
       </c>
       <c r="I51" s="38"/>
+      <c r="J51" s="36" t="s">
+        <v>250</v>
+      </c>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -4944,7 +4971,7 @@
       <c r="B52" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C52" s="69" t="s">
+      <c r="C52" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D52" s="36" t="s">
@@ -4956,7 +4983,7 @@
       <c r="F52" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="G52" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H52" s="35" t="s">
@@ -4974,7 +5001,7 @@
       <c r="B53" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="C53" s="69" t="s">
+      <c r="C53" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D53" s="36" t="s">
@@ -4986,7 +5013,7 @@
       <c r="F53" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G53" s="37" t="s">
+      <c r="G53" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H53" s="35" t="s">
@@ -5004,7 +5031,7 @@
       <c r="B54" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="C54" s="69" t="s">
+      <c r="C54" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D54" s="40" t="s">
@@ -5016,8 +5043,8 @@
       <c r="F54" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G54" s="39" t="s">
-        <v>183</v>
+      <c r="G54" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H54" s="38" t="s">
         <v>77</v>
@@ -5034,7 +5061,7 @@
       <c r="B55" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="C55" s="69" t="s">
+      <c r="C55" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D55" s="40" t="s">
@@ -5046,8 +5073,8 @@
       <c r="F55" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="39" t="s">
-        <v>183</v>
+      <c r="G55" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H55" s="38" t="s">
         <v>77</v>
@@ -5064,7 +5091,7 @@
       <c r="B56" s="35" t="s">
         <v>269</v>
       </c>
-      <c r="C56" s="69" t="s">
+      <c r="C56" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D56" s="36" t="s">
@@ -5076,7 +5103,7 @@
       <c r="F56" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G56" s="37" t="s">
+      <c r="G56" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H56" s="35" t="s">
@@ -5094,7 +5121,7 @@
       <c r="B57" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="C57" s="69" t="s">
+      <c r="C57" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D57" s="36" t="s">
@@ -5106,7 +5133,7 @@
       <c r="F57" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G57" s="37" t="s">
+      <c r="G57" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H57" s="35" t="s">
@@ -5124,7 +5151,7 @@
       <c r="B58" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="C58" s="69" t="s">
+      <c r="C58" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D58" s="40" t="s">
@@ -5136,8 +5163,8 @@
       <c r="F58" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G58" s="39" t="s">
-        <v>183</v>
+      <c r="G58" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H58" s="38" t="s">
         <v>77</v>
@@ -5154,7 +5181,7 @@
       <c r="B59" s="38" t="s">
         <v>272</v>
       </c>
-      <c r="C59" s="69" t="s">
+      <c r="C59" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D59" s="40" t="s">
@@ -5166,8 +5193,8 @@
       <c r="F59" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G59" s="39" t="s">
-        <v>183</v>
+      <c r="G59" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H59" s="38" t="s">
         <v>77</v>
@@ -5184,7 +5211,7 @@
       <c r="B60" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="C60" s="69" t="s">
+      <c r="C60" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D60" s="36" t="s">
@@ -5196,7 +5223,7 @@
       <c r="F60" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G60" s="37" t="s">
+      <c r="G60" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H60" s="35" t="s">
@@ -5214,7 +5241,7 @@
       <c r="B61" s="35" t="s">
         <v>274</v>
       </c>
-      <c r="C61" s="69" t="s">
+      <c r="C61" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D61" s="36" t="s">
@@ -5226,7 +5253,7 @@
       <c r="F61" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G61" s="37" t="s">
+      <c r="G61" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H61" s="35" t="s">
@@ -5244,7 +5271,7 @@
       <c r="B62" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="C62" s="69" t="s">
+      <c r="C62" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D62" s="40" t="s">
@@ -5256,8 +5283,8 @@
       <c r="F62" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G62" s="39" t="s">
-        <v>183</v>
+      <c r="G62" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H62" s="38" t="s">
         <v>77</v>
@@ -5274,7 +5301,7 @@
       <c r="B63" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="C63" s="69" t="s">
+      <c r="C63" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D63" s="40" t="s">
@@ -5286,8 +5313,8 @@
       <c r="F63" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G63" s="39" t="s">
-        <v>183</v>
+      <c r="G63" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H63" s="38" t="s">
         <v>76</v>
@@ -5301,7 +5328,7 @@
       <c r="B64" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="C64" s="69" t="s">
+      <c r="C64" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D64" s="40" t="s">
@@ -5313,8 +5340,8 @@
       <c r="F64" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G64" s="39" t="s">
-        <v>183</v>
+      <c r="G64" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H64" s="38" t="s">
         <v>77</v>
@@ -5331,7 +5358,7 @@
       <c r="B65" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="C65" s="69" t="s">
+      <c r="C65" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D65" s="36" t="s">
@@ -5343,7 +5370,7 @@
       <c r="F65" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="G65" s="37" t="s">
+      <c r="G65" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H65" s="35" t="s">
@@ -5361,7 +5388,7 @@
       <c r="B66" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="C66" s="69" t="s">
+      <c r="C66" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D66" s="36" t="s">
@@ -5373,7 +5400,7 @@
       <c r="F66" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="G66" s="37" t="s">
+      <c r="G66" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H66" s="35" t="s">
@@ -5391,7 +5418,7 @@
       <c r="B67" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="C67" s="69" t="s">
+      <c r="C67" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D67" s="40" t="s">
@@ -5403,8 +5430,8 @@
       <c r="F67" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="39" t="s">
-        <v>183</v>
+      <c r="G67" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H67" s="38" t="s">
         <v>77</v>
@@ -5421,7 +5448,7 @@
       <c r="B68" s="35" t="s">
         <v>300</v>
       </c>
-      <c r="C68" s="69" t="s">
+      <c r="C68" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D68" s="36" t="s">
@@ -5433,7 +5460,7 @@
       <c r="F68" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="G68" s="39" t="s">
+      <c r="G68" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H68" s="35" t="s">
@@ -5451,7 +5478,7 @@
       <c r="B69" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="C69" s="69" t="s">
+      <c r="C69" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D69" s="40" t="s">
@@ -5463,8 +5490,8 @@
       <c r="F69" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G69" s="39" t="s">
-        <v>183</v>
+      <c r="G69" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H69" s="38" t="s">
         <v>77</v>
@@ -5478,7 +5505,7 @@
       <c r="B70" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="C70" s="69" t="s">
+      <c r="C70" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D70" s="40" t="s">
@@ -5488,10 +5515,10 @@
         <v>418</v>
       </c>
       <c r="F70" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G70" s="39" t="s">
-        <v>183</v>
+        <v>464</v>
+      </c>
+      <c r="G70" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H70" s="38" t="s">
         <v>77</v>
@@ -5505,7 +5532,7 @@
       <c r="B71" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="C71" s="69" t="s">
+      <c r="C71" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D71" s="40" t="s">
@@ -5515,10 +5542,10 @@
         <v>418</v>
       </c>
       <c r="F71" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G71" s="39" t="s">
-        <v>183</v>
+        <v>464</v>
+      </c>
+      <c r="G71" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H71" s="38" t="s">
         <v>77</v>
@@ -5532,7 +5559,7 @@
       <c r="B72" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="C72" s="69" t="s">
+      <c r="C72" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D72" s="40" t="s">
@@ -5542,10 +5569,10 @@
         <v>418</v>
       </c>
       <c r="F72" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G72" s="39" t="s">
-        <v>183</v>
+        <v>464</v>
+      </c>
+      <c r="G72" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H72" s="38" t="s">
         <v>77</v>
@@ -5559,7 +5586,7 @@
       <c r="B73" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="C73" s="69" t="s">
+      <c r="C73" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D73" s="40" t="s">
@@ -5571,8 +5598,8 @@
       <c r="F73" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G73" s="39" t="s">
-        <v>183</v>
+      <c r="G73" s="41" t="s">
+        <v>327</v>
       </c>
       <c r="H73" s="38" t="s">
         <v>77</v>
@@ -5586,7 +5613,7 @@
       <c r="B74" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C74" s="69" t="s">
+      <c r="C74" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D74" s="40" t="s">
@@ -5596,9 +5623,9 @@
         <v>418</v>
       </c>
       <c r="F74" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G74" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="G74" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H74" s="38" t="s">
@@ -5613,7 +5640,7 @@
       <c r="B75" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="C75" s="69" t="s">
+      <c r="C75" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D75" s="40" t="s">
@@ -5623,9 +5650,9 @@
         <v>418</v>
       </c>
       <c r="F75" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G75" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="G75" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H75" s="38" t="s">
@@ -5640,7 +5667,7 @@
       <c r="B76" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="C76" s="69" t="s">
+      <c r="C76" s="53" t="s">
         <v>417</v>
       </c>
       <c r="D76" s="40" t="s">
@@ -5650,9 +5677,9 @@
         <v>418</v>
       </c>
       <c r="F76" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G76" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="G76" s="55" t="s">
         <v>183</v>
       </c>
       <c r="H76" s="38" t="s">
@@ -5662,7 +5689,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G63:G64 G46:G50 G5:G42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G76">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5759,452 +5786,452 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+    <row r="5" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="43" t="s">
         <v>327</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-    </row>
-    <row r="6" spans="1:11" s="63" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="G5" s="42"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+    </row>
+    <row r="6" spans="1:11" s="47" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
         <v>330</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="42" t="s">
         <v>329</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43" t="s">
         <v>327</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-    </row>
-    <row r="7" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="G6" s="42"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+    </row>
+    <row r="7" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="43" t="s">
         <v>327</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-    </row>
-    <row r="8" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="G7" s="42"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+    </row>
+    <row r="8" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
         <v>345</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="42" t="s">
         <v>349</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58" t="s">
+      <c r="C8" s="42"/>
+      <c r="D8" s="42" t="s">
         <v>353</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-    </row>
-    <row r="9" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="E8" s="43"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+    </row>
+    <row r="9" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
         <v>346</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="42" t="s">
         <v>350</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="E9" s="59"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-    </row>
-    <row r="10" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="E9" s="43"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+    </row>
+    <row r="10" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58" t="s">
+      <c r="C10" s="42"/>
+      <c r="D10" s="42" t="s">
         <v>355</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-    </row>
-    <row r="11" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+    </row>
+    <row r="11" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="42" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-    </row>
-    <row r="12" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="E11" s="43"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+    </row>
+    <row r="12" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
         <v>338</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="42" t="s">
         <v>342</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58" t="s">
+      <c r="C12" s="42"/>
+      <c r="D12" s="42" t="s">
         <v>335</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-    </row>
-    <row r="13" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="E12" s="43"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+    </row>
+    <row r="13" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
         <v>339</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="42" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58" t="s">
+      <c r="C13" s="42"/>
+      <c r="D13" s="42" t="s">
         <v>336</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-    </row>
-    <row r="14" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="E13" s="43"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+    </row>
+    <row r="14" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
         <v>340</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="42" t="s">
         <v>344</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="42" t="s">
         <v>337</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
-    </row>
-    <row r="15" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+    </row>
+    <row r="15" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
         <v>365</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="60" t="s">
+      <c r="C15" s="42"/>
+      <c r="D15" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-    </row>
-    <row r="16" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="E15" s="43"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+    </row>
+    <row r="16" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
         <v>366</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="60" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-    </row>
-    <row r="17" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="58" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+    </row>
+    <row r="17" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
         <v>367</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="42" t="s">
         <v>359</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="60" t="s">
+      <c r="C17" s="42"/>
+      <c r="D17" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-    </row>
-    <row r="18" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="E17" s="43"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+    </row>
+    <row r="18" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
         <v>368</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="42" t="s">
         <v>360</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="60" t="s">
+      <c r="C18" s="42"/>
+      <c r="D18" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
-    </row>
-    <row r="19" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+    </row>
+    <row r="19" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
         <v>372</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="60" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="E19" s="59"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
-    </row>
-    <row r="20" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="E19" s="43"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+    </row>
+    <row r="20" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
         <v>373</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="42" t="s">
         <v>362</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="60" t="s">
+      <c r="C20" s="42"/>
+      <c r="D20" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="E20" s="59"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-    </row>
-    <row r="21" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+      <c r="E20" s="43"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+    </row>
+    <row r="21" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
         <v>374</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="42" t="s">
         <v>363</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="60" t="s">
+      <c r="C21" s="42"/>
+      <c r="D21" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="E21" s="59"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-    </row>
-    <row r="22" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="E21" s="43"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+    </row>
+    <row r="22" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>375</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="42" t="s">
         <v>364</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="60" t="s">
+      <c r="C22" s="42"/>
+      <c r="D22" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
-    </row>
-    <row r="23" spans="1:11" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
+      <c r="E22" s="43"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+    </row>
+    <row r="23" spans="1:11" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
         <v>379</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="42" t="s">
         <v>376</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="60" t="s">
+      <c r="C23" s="42"/>
+      <c r="D23" s="44" t="s">
         <v>378</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-    </row>
-    <row r="24" spans="1:11" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="E23" s="43"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+    </row>
+    <row r="24" spans="1:11" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="42" t="s">
         <v>377</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="60" t="s">
+      <c r="C24" s="42"/>
+      <c r="D24" s="44" t="s">
         <v>378</v>
       </c>
-      <c r="E24" s="59"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-    </row>
-    <row r="25" spans="1:11" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
+      <c r="E24" s="43"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+    </row>
+    <row r="25" spans="1:11" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="42" t="s">
         <v>383</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="60" t="s">
+      <c r="C25" s="42"/>
+      <c r="D25" s="44" t="s">
         <v>386</v>
       </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-    </row>
-    <row r="26" spans="1:11" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="E25" s="43"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+    </row>
+    <row r="26" spans="1:11" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
         <v>385</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="48" t="s">
         <v>381</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="60" t="s">
+      <c r="C26" s="42"/>
+      <c r="D26" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="59"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-    </row>
-    <row r="27" spans="1:11" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
+      <c r="E26" s="43"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+    </row>
+    <row r="27" spans="1:11" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="42" t="s">
         <v>413</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="58" t="s">
+      <c r="C27" s="49"/>
+      <c r="D27" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="59"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
     </row>
     <row r="28" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
@@ -7098,15 +7125,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="56"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -7172,15 +7199,15 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="74"/>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -7246,15 +7273,15 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="74"/>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
@@ -7425,15 +7452,15 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="56"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
     </row>
     <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
@@ -7619,15 +7646,15 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="56"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -7723,15 +7750,15 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="74"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -7833,15 +7860,15 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="74"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -8135,15 +8162,15 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="56"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="74"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>

</xml_diff>

<commit_message>
create test cases Postman
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="811">
   <si>
     <t>ID</t>
   </si>
@@ -2223,6 +2223,9 @@
     <t xml:space="preserve"> arina.</t>
   </si>
   <si>
+    <t xml:space="preserve">.arina </t>
+  </si>
+  <si>
     <t>arina..</t>
   </si>
   <si>
@@ -2242,9 +2245,6 @@
   </si>
   <si>
     <t xml:space="preserve"> strashchenko_</t>
-  </si>
-  <si>
-    <t>-strashchenko</t>
   </si>
   <si>
     <t>strashchenko''</t>
@@ -2721,6 +2721,21 @@
   <si>
     <t xml:space="preserve">Arinaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa
 </t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>"Arina",s,straschenko13@mail.ru,tDbb@58!</t>
   </si>
 </sst>
 </file>
@@ -7373,7 +7388,7 @@
   <dimension ref="A1:L128"/>
   <sheetViews>
     <sheetView topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:D58"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12206,10 +12221,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12223,16 +12238,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="62" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>32</v>
+        <v>806</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>108</v>
+        <v>807</v>
       </c>
       <c r="C1" s="78" t="s">
-        <v>33</v>
+        <v>808</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>34</v>
+        <v>809</v>
       </c>
       <c r="E1" s="69"/>
     </row>
@@ -12378,7 +12393,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="40" t="s">
+        <v>643</v>
+      </c>
       <c r="B12" s="41" t="s">
         <v>692</v>
       </c>
@@ -12391,7 +12408,7 @@
     </row>
     <row r="13" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B13" s="41" t="s">
         <v>692</v>
@@ -12405,7 +12422,7 @@
     </row>
     <row r="14" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B14" s="41" t="s">
         <v>692</v>
@@ -12436,7 +12453,7 @@
         <v>691</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C16" s="79" t="s">
         <v>668</v>
@@ -12445,12 +12462,12 @@
         <v>682</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
         <v>691</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C17" s="79" t="s">
         <v>668</v>
@@ -12459,12 +12476,12 @@
         <v>682</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
         <v>691</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C18" s="79" t="s">
         <v>668</v>
@@ -12473,7 +12490,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
         <v>691</v>
       </c>
@@ -12487,7 +12504,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
         <v>691</v>
       </c>
@@ -12501,7 +12518,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
         <v>691</v>
       </c>
@@ -12515,7 +12532,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>691</v>
       </c>
@@ -12529,12 +12546,12 @@
         <v>682</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>691</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C23" s="79" t="s">
         <v>668</v>
@@ -12543,12 +12560,12 @@
         <v>682</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>691</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C24" s="79" t="s">
         <v>668</v>
@@ -12557,13 +12574,11 @@
         <v>682</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>691</v>
       </c>
-      <c r="B25" s="40" t="s">
-        <v>650</v>
-      </c>
+      <c r="B25" s="40"/>
       <c r="C25" s="79" t="s">
         <v>668</v>
       </c>
@@ -12571,7 +12586,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>691</v>
       </c>
@@ -12585,7 +12600,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>691</v>
       </c>
@@ -12599,7 +12614,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>691</v>
       </c>
@@ -12610,8 +12625,11 @@
       <c r="D28" s="41" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="69" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>691</v>
       </c>
@@ -12625,7 +12643,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="62" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="62" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>691</v>
       </c>
@@ -12640,7 +12658,7 @@
       </c>
       <c r="E30" s="69"/>
     </row>
-    <row r="31" spans="1:5" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
         <v>691</v>
       </c>
@@ -12655,7 +12673,7 @@
       </c>
       <c r="E31" s="99"/>
     </row>
-    <row r="32" spans="1:5" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>691</v>
       </c>
@@ -12752,7 +12770,7 @@
       <c r="B38" s="41" t="s">
         <v>692</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="65" t="s">
         <v>795</v>
       </c>
       <c r="D38" s="41" t="s">
@@ -13310,9 +13328,10 @@
     <hyperlink ref="C64:C75" r:id="rId3" display="straschenko13@mail.ru"/>
     <hyperlink ref="C2" r:id="rId4"/>
     <hyperlink ref="C15" r:id="rId5"/>
+    <hyperlink ref="C38" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update test cases Postman
</commit_message>
<xml_diff>
--- a/Web_Form_Testing.xlsx
+++ b/Web_Form_Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Требования" sheetId="1" r:id="rId1"/>
@@ -4305,8 +4305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B61" sqref="B59:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7387,8 +7387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12223,8 +12223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13133,7 +13133,7 @@
       <c r="C62" s="40" t="s">
         <v>679</v>
       </c>
-      <c r="D62" s="41" t="s">
+      <c r="D62" s="52" t="s">
         <v>682</v>
       </c>
       <c r="E62" s="99"/>
@@ -13329,9 +13329,10 @@
     <hyperlink ref="C2" r:id="rId4"/>
     <hyperlink ref="C15" r:id="rId5"/>
     <hyperlink ref="C38" r:id="rId6"/>
+    <hyperlink ref="D62" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>